<commit_message>
Moved fixesandfeatures into README Allowed JSON data fixed CSV data read-in Allow each section to have its own data file
</commit_message>
<xml_diff>
--- a/example/cvdata.xlsx
+++ b/example/cvdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nhuntington-klein\Dropbox (CSU Fullerton)\AutoCV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nhuntington-klein\Dropbox (CSU Fullerton)\CVRoller\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="134">
   <si>
     <t>section</t>
   </si>
@@ -95,39 +95,9 @@
     <t>B.A. in Economics and Mathematics, Reed College, 2009</t>
   </si>
   <si>
-    <t>cites</t>
-  </si>
-  <si>
     <t>pubs2</t>
   </si>
   <si>
-    <t xml:space="preserve">Huntington-Klein, Nick. 2015. "Subjective and Projected Returns to Education" *Journal of Economic Behavior &amp; Organization*. 117, p. 10-25. </t>
-  </si>
-  <si>
-    <t>Long, Mark C., Dan Goldhaber, &amp; Nick Huntington-Klein. 2015. "Do Completed College Majors Respond to Changes in Wages?" *Economics of Education Review*. 49, p. 1-14.</t>
-  </si>
-  <si>
-    <t>Huntington-Klein, Nick. 2016. "’(Un)informed College and Major Choice’: Verification in an Alternate Setting" *Economics of Education Review*. 53, p. 159-163.</t>
-  </si>
-  <si>
-    <t>Huntington-Klein, Nick. 2017. "A Method for Estimating Local Average Treatment Effects in Aggregate Data with Imperfect Assignment" *Applied Economics Letters*. 24(11), p. 762-765.</t>
-  </si>
-  <si>
-    <t>Huntington-Klein, Nick, James Cowan, &amp; Dan Goldhaber. 2017. "Selection into Online Community College Courses and their Effects on Persistence" *Research in Higher Education*. 58(3), p. 244-269</t>
-  </si>
-  <si>
-    <t>Goldhaber, Dan., Cyrus Grout, &amp; Nick Huntington-Klein. 2017. "Screen Twice, Cut Once: Assessing the Predictive Validity of Applicant Selection Tools" *Education Finance and Policy*. 12(2), p. 197-223</t>
-  </si>
-  <si>
-    <t>Huntington-Klein, Nick. 2018. "College Choice as a Collective Decision" *Economic Inquiry*. 56(2), p. 1202-1219.</t>
-  </si>
-  <si>
-    <t>Huntington-Klein, Nick and Elaina Rose. 2018. "Peer Effects in a Predominantly Male Environment: Evidence from West Point" *AEA Papers and Proceedings*. 108, p. 392-395.</t>
-  </si>
-  <si>
-    <t>Huntington-Klein, Nick and Elizabeth Ackert. 2018. "The Long Road to Equality: A Meta-analysis of the Influence of African American Racial Status on Student Achievement over Time" *Social Science Quarterly*. 99(3), p.1119-1133.</t>
-  </si>
-  <si>
     <t>"vtable: A Quick and Easy Variable Browser for R." 2018. [github.com/NickCH-K/vtable](github.com/NickCH-K/vtable).</t>
   </si>
   <si>
@@ -152,69 +122,12 @@
     <t>abstract</t>
   </si>
   <si>
-    <t>There is significant heterogeneity over high school students in the wage and employment rate returns to education. I evaluate this heterogeneity using subjective returns derived from a data set of high school juniors and seniors in Washington State. Variation over observables in projected returns estimated using observed data is uncorrelated with variation in subjective returns elicited by directly asking students about their beliefs. These results mean that returns estimated using observed data are likely a very weak proxy for student beliefs.</t>
-  </si>
-  <si>
     <t>link</t>
   </si>
   <si>
-    <t>http://www.sciencedirect.com/science/article/pii/S0167268115001407</t>
-  </si>
-  <si>
     <t>extra</t>
   </si>
   <si>
-    <t>Recipient of 2013 Storer Award for Labor Economics.</t>
-  </si>
-  <si>
-    <t>http://www.sciencedirect.com/science/article/pii/S027277571500103X</t>
-  </si>
-  <si>
-    <t>http://www.sciencedirect.com/science/article/pii/S0272775715302284</t>
-  </si>
-  <si>
-    <t>In some contexts, the effect of a treatment can be estimated with easily-accessible aggregate rather than individual data, using difference-in-difference estimation. However, under imperfect assignment this produces intent-to-treat estimates, which may not be the treatment effect of interest. This paper provides a method for estimating local average treatment effects using aggregate data. I also suggest a data source that allows the method to be applied when treatment rates are not recorded.</t>
-  </si>
-  <si>
-    <t>http://www.tandfonline.com/doi/full/10.1080/13504851.2016.1226483</t>
-  </si>
-  <si>
-    <t>Online courses at the college level are growing in popularity, and nearly all community colleges offer online courses (Allen &amp; Seaman, 2015). What is the effect of the expanded availability of online curricula on persistence in the field and towards a degree? We use a model of self-selection to estimate the effect of taking an online course, using region and time variation in internet service as a source of identifying variation. Our method, as opposed to standard experimental methods, allows us to consider the effect among students who actually choose to take such courses. For the average person, taking an online course has a negative effect on the probability of taking another course in the same field and on the probability of earning a degree. The negative effect on graduation for for students who choose to take an online course is stronger than the negative effect for the average student. Community colleges must balance these results against the attractive features of online courses, and may want to consider actively targeting online courses towards those most likely to do well in them.</t>
-  </si>
-  <si>
-    <t>http://link.springer.com/article/10.1007/s11162-016-9425-z</t>
-  </si>
-  <si>
-    <t>Despite their widespread use, there is little academic evidence on whether applicant selection tools can improve teacher-hiring processes. We examine two screening instruments used to select classroom teachers. The screening instruments strongly predict teacher value-added in math and teacher attrition and weakly predict value-added in reading, but do not predict teacher absences. An increase of one standard deviation in screening scores is associated with an increase of about 0.06 standard deviations of student math achievement and a decrease in teacher attrition of three percentage points. These results are robust to corrections for sample selection.</t>
-  </si>
-  <si>
-    <t>http://www.mitpressjournals.org/doi/abs/10.1162/EDFP_a_00200#.V-AgX_lpEdV</t>
-  </si>
-  <si>
-    <t>Although the choice between colleges can be thought of as being made collectively by a family, models of educational choice almost universally portray the decision as made by the student alone. Using a novel experimental method for identifying collective decision functions, I find that students have more influence than parents over the decision, but not exclusive control. Students care more than parents about classroom experience and future earnings. Ignoring the dual-agent nature of the decision can weaken predictions and lead to poorly-targeted policy designs.</t>
-  </si>
-  <si>
-    <t>http://onlinelibrary.wiley.com/doi/10.1111/ecin.12470/full</t>
-  </si>
-  <si>
-    <t>[Working Paper PDF](http://nickchk.com/Huntington-Klein_2017_College_Choice_as_a_Collective_Decision.pdf)</t>
-  </si>
-  <si>
-    <t>The last several decades have seen a dramatic increase in the representation of women in traditionally male professions (e.g. Goldin 2014). Growth has been slower among Science/Technology/Engineering/Math (STEM) fields and military officers. Economists have paid much attention to the former, far less to the latter. Explanations include (Bertrand et al. 2010). The literature on female performance in these areas is wide, but many descriptive studies support to some degree the commonly held belief that women with women peers and mentors are more likely to enter and persist in male-advantaged environments (e.g. Drury et al. 2011; Flabbi et al. 2012; Kunze &amp; Miller 2014). These studies are limited, as standard issues with peer and mentor effects studies apply, including the endogenous selection of group. This paper follows previous work recognizing that random assignment of cadets (students) to companies and classes at military academies can help inform our understanding of interactions in broader contexts (Lyle 2007; Carrell et al. 2008). We extend Lyle's (2007) work by estimating gender-specific peer and mentor effects and focus on retention of women at West Point in the first years in which women were admitted. We find that women do significantly better when placed in companies with more women peers. The addition of one woman peer is predicted to reduce the gender progression gap by half. We see no effect of peer gender on the retention of men.</t>
-  </si>
-  <si>
-    <t>https://www.aeaweb.org/articles?id=10.1257/pandp.20181114</t>
-  </si>
-  <si>
-    <t>This study performs a meta-regression analysis of over 1,100 regressions in 165 studies to examine the relationship between African American racial status and student achievement scores in K-12 education from 1979 to 2010. The study examines time trends in the black test score gap and estimates the extent to which controls for confounding variables including socioeconomic status and schooling characteristics attenuate the size of the gap. Across the samples in the study, the absolute relationship between Black status and achievement decreased during the 1980s and early 1990s, but has been stagnant since the late 1990s. We estimate that socioeconomic status alone explains more than half of the gap, and this influence does not vary significantly over the time period of interest. Controlling for differences in school characteristics only reduces the gap slightly, but school-level factors explain an increasing proportion of the gap over time.</t>
-  </si>
-  <si>
-    <t>https://onlinelibrary.wiley.com/doi/abs/10.1111/ssqu.12483</t>
-  </si>
-  <si>
-    <t>[Working Paper PDF](http://nickchk.com/Huntington-Klein_Ackert_Full_Long_Road_to_Equality.pdf). [Online Appendices](http://nickchk.com/Huntington-Klein_Ackert_SSQ_Appendices.pdf).</t>
-  </si>
-  <si>
     <t>"A Study of West Point Shows How Women Help Each Other Advance" with Elaina Rose (2018). Harvard Business Review.</t>
   </si>
   <si>
@@ -275,9 +188,6 @@
     <t>"Most Likely to Succeed: Personality and Long-Run Economic Outcomes" with Elaina Rose.</t>
   </si>
   <si>
-    <t>"Human Capital vs. Signaling is Empirically Unresolvable" (2018). CSUF Department of Economics Working Paper 2018/010.</t>
-  </si>
-  <si>
     <t>Economists offer two major explanations for the fact that we find causal labor market returns to education. The first is human capital accumulation: education improves ability. The second is signaling: education allows initially high-ability students to distinguish themselves. A major point of interest in the economics of education is relative contributions of signaling and human capital. Empirical evidence generally excludes the trivial case: neither human capital nor signaling explain either 0% or 100% of the return. I argue that exclusions of the trivial case form the limits of what can be learned from empirical data. An education returns model with some non-zero contribution of both signaling and human capital cannot be empirically distinguished from another model with different non-zero contributions, making human capital vs. signaling a poor framing for understanding the return as a whole, and for policy decision-making.</t>
   </si>
   <si>
@@ -494,60 +404,6 @@
     <t>Huntington-Klein, Nick. 2018. "A Step-by-Step Guide to the Principles of Microeconomics." Kona Publishing.</t>
   </si>
   <si>
-    <t>media</t>
-  </si>
-  <si>
-    <t>Findings on Education Finance and Policy Discussed by Investigators at University of Washington. Education Letter, May 3 2017</t>
-  </si>
-  <si>
-    <t>[Chico's, Unilever GSK, 'Handmaid's Tale' Sequel: Broadsheet November 29](http://fortune.com/2018/11/29/chicos-unilever-gsk-handmaids-tale-sequel-broadsheet-november-29/?xid=gn_editorspicks). Fortune Magazine, December 1, 2018</t>
-  </si>
-  <si>
-    <t>[The faiV: Week of November 26, 2018: The Astounding Edition](https://mailchi.mp/financialaccess/the-faiv-week-of-nov262018). fai, November 30, 2018</t>
-  </si>
-  <si>
-    <t>[High-Five Your Work Wife: New Study Shows How Women Help Each Other Advance](https://www.purewow.com/news/west-point-study-on-women-helping-each-other-at-work). PureWow, Sarah Stiefvater, November 29, 2018</t>
-  </si>
-  <si>
-    <t>[On Caplan Educational Signaling (#6)](https://marginalrevolution.com/marginalrevolution/2018/11/tuesday-assorted-links-191.html). Tuesday Assorted Links, Marginal Revoluation, November 27, 2018</t>
-  </si>
-  <si>
-    <t>[Killing Colleges in Massachusetts](https://www.insidehighered.com/views/2018/08/29/state-policy-makers-should-stop-overlooking-role-private-colleges-providing-access). Inside Higher Ed, August 29, 2018</t>
-  </si>
-  <si>
-    <t>[Cal State Fullerton professor wonders whether major course requirements could be made simpler](https://dailytitan.com/2018/02/cal-state-fullerton-professor-wonders-whether-major-course-requirements-made-simpler/). The Daily Titan, February 26, 2018</t>
-  </si>
-  <si>
-    <t>[Private colleges can partner to solve issues](http://www.theintelligencer.com/news/article/Private-colleges-can-partner-to-solve-issues-11129681.php). The Edwardsville Intelligencer, May 8, 2017</t>
-  </si>
-  <si>
-    <t>[The Value of a College Degree](http://www.theintermountain.com/opinion/columnists/2017/04/the-value-of-a-college-degree/). The Inter-Mountain, April 27, 2017</t>
-  </si>
-  <si>
-    <t>[Incentives to Attend Private Colleges Could Save States Money and Raise Graduation Rates](http://www.chronicle.com/article/Incentives-to-Attend-Private/239801?cid=at&amp;utm_source=at&amp;utm_medium=en&amp;elqTrackId=5719cd9ce29549cf9b399520678c52f0&amp;elq=c46d8f380cc14466861c12899b770d6c&amp;elqaid=13488&amp;elqat=1&amp;elqCampaignId=5599). The Chronicle of Higher Education, April 14, 2017</t>
-  </si>
-  <si>
-    <t>[Hiring Successful Teachers - Two New Studies Point to What Works and What Doesn't](https://www.edsurge.com/news/2016-10-03-hiring-successful-teachers-two-new-studies-point-to-what-works-and-what-doesn-t). EdSurge, October 3, 2016</t>
-  </si>
-  <si>
-    <t>[CSUF researcher studies how stereotypes affect higher education decisions](http://www.ocregister.com/articles/college-715504-students-klein.html). OC Register, May 12, 2016</t>
-  </si>
-  <si>
-    <t>[How Will Your College Degree Pay Off?](https://bizblogs.fullerton.edu/blog/2016/01/04/how-will-your-college-degree-pay-off/) Mihaylo College Bizblog, January 4, 2016</t>
-  </si>
-  <si>
-    <t>[Facing growing scrutiny, colleges set out to prove their value](http://hechingerreport.org/25399-2/). The Hechinger Report, January 22, 2016.</t>
-  </si>
-  <si>
-    <t>[Is Robert anti-teacher?](https://edexcellence.net/commentary/podcasts/is-robert-anti-teacher) The Education Gadfly, November 5, 2014</t>
-  </si>
-  <si>
-    <t>[Study: Teacher hiring should be more scientific](http://komonews.com/news/local/study-teacher-hiring-should-be-more-scientific). Associated Press, October 29, 2014</t>
-  </si>
-  <si>
-    <t>In an analysis connecting labor market earnings to college major choices, we find statistically significant relationships between changes in wages by occupation and subsequent changes in college majors completed in related fields of college study between 1982 and 2012. College majors (defined at a detailed level) are most strongly related to wages observed three years earlier, when students were college freshmen. The responses to wages vary depending on the extent to which there is a strong mapping of majors into particular occupations. We also find that women, blacks, Hispanics, and students with low test scores are less likely to respond to wage changes. These findings have implications for policy interventions designed to align students' major choices with labor market demand.</t>
-  </si>
-  <si>
     <t>workingon</t>
   </si>
   <si>
@@ -570,9 +426,6 @@
   </si>
   <si>
     <t>"Human Capital vs. Signaling is Empirically Unresolvable." CSU Fullerton Department of Economics Working Paper 2018/010.</t>
-  </si>
-  <si>
-    <t>In their recent paper "(Un)informed College and Major Choice: Evidence from Linked Survey and Administrative Data," Hastings, Neilson, Ramirez, &amp; Zimmerman (2016) provide an informal costly-information model, linking family background to students' beliefs about educational costs and benefits. They verify predictions of their model using a data set of beliefs about college institutions and majors among Chilean college applicants and students. I test some of those same predictions using a data set of beliefs about college institutions and different levels of college education among high school students in the United States. I verify their predictions, with some exceptions, supporting the use of their costly-search model.</t>
   </si>
 </sst>
 </file>
@@ -903,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D163"/>
+  <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,7 +772,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1054,13 +907,13 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1068,13 +921,13 @@
         <v>23</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1082,13 +935,13 @@
         <v>23</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1096,13 +949,13 @@
         <v>23</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1110,13 +963,13 @@
         <v>23</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1124,13 +977,13 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>173</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1138,13 +991,13 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1152,13 +1005,13 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1166,13 +1019,13 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>182</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1180,13 +1033,13 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1194,13 +1047,13 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1208,13 +1061,13 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1222,13 +1075,13 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" t="s">
         <v>43</v>
-      </c>
-      <c r="D25" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1236,13 +1089,13 @@
         <v>23</v>
       </c>
       <c r="B26">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1250,13 +1103,13 @@
         <v>23</v>
       </c>
       <c r="B27">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D27" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1264,13 +1117,13 @@
         <v>23</v>
       </c>
       <c r="B28">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1278,13 +1131,13 @@
         <v>23</v>
       </c>
       <c r="B29">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1292,13 +1145,13 @@
         <v>23</v>
       </c>
       <c r="B30">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D30" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1306,13 +1159,13 @@
         <v>23</v>
       </c>
       <c r="B31">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1320,13 +1173,13 @@
         <v>23</v>
       </c>
       <c r="B32">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1334,729 +1187,669 @@
         <v>23</v>
       </c>
       <c r="B33">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D33" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B34">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B35">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B36">
         <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D36" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B37">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D37" t="s">
-        <v>58</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B38">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D38" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B39">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>40</v>
-      </c>
-      <c r="D39" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="D39" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B40">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D40" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B41">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>43</v>
-      </c>
-      <c r="D41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B42">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>45</v>
-      </c>
-      <c r="D42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B43">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D43" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B44">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B45">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B46">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D46" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B47">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B48">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C48" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D48" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B49">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C49" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D49" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B50">
-        <v>4.5</v>
+        <v>10</v>
       </c>
       <c r="C50" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D50" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>24</v>
-      </c>
-      <c r="B51">
-        <v>4.5</v>
-      </c>
-      <c r="C51" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="D51" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B52">
-        <v>4.5</v>
-      </c>
-      <c r="C52" t="s">
-        <v>45</v>
-      </c>
-      <c r="D52" t="s">
-        <v>70</v>
+        <v>5</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B53">
-        <v>3</v>
-      </c>
-      <c r="C53" t="s">
-        <v>40</v>
-      </c>
-      <c r="D53" t="s">
-        <v>37</v>
+        <v>4</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B54">
         <v>3</v>
       </c>
-      <c r="C54" t="s">
-        <v>41</v>
-      </c>
-      <c r="D54" t="s">
-        <v>71</v>
+      <c r="D54" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B55">
-        <v>3</v>
-      </c>
-      <c r="C55" t="s">
-        <v>45</v>
-      </c>
-      <c r="D55" t="s">
-        <v>72</v>
+        <v>2</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B56">
-        <v>2</v>
-      </c>
-      <c r="C56" t="s">
-        <v>40</v>
-      </c>
-      <c r="D56" t="s">
-        <v>38</v>
+        <v>1</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="B57">
-        <v>2</v>
-      </c>
-      <c r="C57" t="s">
-        <v>41</v>
-      </c>
-      <c r="D57" t="s">
-        <v>73</v>
+        <v>10</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="B58">
-        <v>1</v>
-      </c>
-      <c r="C58" t="s">
-        <v>40</v>
-      </c>
-      <c r="D58" t="s">
-        <v>39</v>
+        <v>9</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="B59">
-        <v>1</v>
-      </c>
-      <c r="C59" t="s">
-        <v>41</v>
-      </c>
-      <c r="D59" t="s">
-        <v>74</v>
+        <v>8</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="B60">
-        <v>1</v>
-      </c>
-      <c r="C60" t="s">
-        <v>43</v>
-      </c>
-      <c r="D60" t="s">
-        <v>75</v>
+        <v>7</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="B61">
-        <v>8</v>
-      </c>
-      <c r="C61" t="s">
-        <v>40</v>
-      </c>
-      <c r="D61" t="s">
-        <v>63</v>
+        <v>6</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="B62">
-        <v>8</v>
-      </c>
-      <c r="C62" t="s">
-        <v>41</v>
-      </c>
-      <c r="D62" t="s">
-        <v>76</v>
+        <v>5</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="B63">
-        <v>8</v>
-      </c>
-      <c r="C63" t="s">
-        <v>43</v>
-      </c>
-      <c r="D63" t="s">
-        <v>77</v>
+        <v>4</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B64">
-        <v>8</v>
-      </c>
-      <c r="C64" t="s">
-        <v>40</v>
-      </c>
-      <c r="D64" t="s">
-        <v>79</v>
+        <v>3</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B65">
-        <v>8</v>
-      </c>
-      <c r="C65" t="s">
-        <v>41</v>
-      </c>
-      <c r="D65" t="s">
-        <v>89</v>
+        <v>2</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B66">
-        <v>8</v>
-      </c>
-      <c r="C66" t="s">
-        <v>45</v>
-      </c>
-      <c r="D66" t="s">
-        <v>90</v>
+        <v>1</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B67">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>40</v>
-      </c>
-      <c r="D67" t="s">
-        <v>181</v>
+        <v>4</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B68">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>41</v>
-      </c>
-      <c r="D68" t="s">
-        <v>84</v>
+        <v>86</v>
+      </c>
+      <c r="D68" s="1">
+        <v>2018</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B69">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C69" t="s">
-        <v>45</v>
-      </c>
-      <c r="D69" t="s">
-        <v>85</v>
+        <v>4</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B70">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C70" t="s">
-        <v>40</v>
-      </c>
-      <c r="D70" t="s">
-        <v>80</v>
+        <v>86</v>
+      </c>
+      <c r="D70" s="1">
+        <v>2018</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B71">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>41</v>
-      </c>
-      <c r="D71" t="s">
-        <v>91</v>
+        <v>4</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B72">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>45</v>
-      </c>
-      <c r="D72" t="s">
-        <v>92</v>
+        <v>86</v>
+      </c>
+      <c r="D72" s="1">
+        <v>2017</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B73">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>40</v>
-      </c>
-      <c r="D73" t="s">
-        <v>81</v>
+        <v>4</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B74">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>41</v>
-      </c>
-      <c r="D74" t="s">
-        <v>93</v>
+        <v>86</v>
+      </c>
+      <c r="D74" s="1">
+        <v>2016</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B75">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C75" t="s">
-        <v>45</v>
-      </c>
-      <c r="D75" t="s">
-        <v>94</v>
+        <v>4</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B76">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C76" t="s">
-        <v>40</v>
-      </c>
-      <c r="D76" t="s">
-        <v>82</v>
+        <v>86</v>
+      </c>
+      <c r="D76" s="1">
+        <v>2014</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B77">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C77" t="s">
-        <v>41</v>
-      </c>
-      <c r="D77" t="s">
-        <v>95</v>
+        <v>4</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B78">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C78" t="s">
-        <v>40</v>
-      </c>
-      <c r="D78" t="s">
-        <v>83</v>
+        <v>86</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B79">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C79" t="s">
-        <v>41</v>
-      </c>
-      <c r="D79" t="s">
-        <v>84</v>
+        <v>4</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B80">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C80" t="s">
-        <v>45</v>
-      </c>
-      <c r="D80" t="s">
-        <v>85</v>
+        <v>86</v>
+      </c>
+      <c r="D80" s="1">
+        <v>2013</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B81">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C81" t="s">
-        <v>40</v>
-      </c>
-      <c r="D81" t="s">
-        <v>86</v>
+        <v>4</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B82">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C82" t="s">
-        <v>41</v>
-      </c>
-      <c r="D82" t="s">
-        <v>88</v>
+        <v>86</v>
+      </c>
+      <c r="D82">
+        <v>2011</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>78</v>
-      </c>
-      <c r="B83">
-        <v>10</v>
-      </c>
-      <c r="C83" t="s">
-        <v>45</v>
-      </c>
-      <c r="D83" t="s">
-        <v>87</v>
+        <v>111</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>96</v>
-      </c>
-      <c r="D84" t="s">
-        <v>155</v>
+        <v>111</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>97</v>
-      </c>
-      <c r="B85">
-        <v>5</v>
+        <v>111</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>98</v>
@@ -2064,10 +1857,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>97</v>
-      </c>
-      <c r="B86">
-        <v>4</v>
+        <v>111</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>99</v>
@@ -2075,10 +1865,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>97</v>
-      </c>
-      <c r="B87">
-        <v>3</v>
+        <v>111</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>100</v>
@@ -2086,10 +1873,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>97</v>
-      </c>
-      <c r="B88">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>101</v>
@@ -2097,10 +1881,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>97</v>
-      </c>
-      <c r="B89">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>102</v>
@@ -2108,753 +1889,235 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>111</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="B90">
-        <v>10</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>103</v>
-      </c>
-      <c r="B91">
-        <v>9</v>
+        <v>111</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>103</v>
-      </c>
-      <c r="B92">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>103</v>
-      </c>
-      <c r="B93">
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>103</v>
-      </c>
-      <c r="B94">
-        <v>6</v>
+        <v>111</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>103</v>
-      </c>
-      <c r="B95">
-        <v>5</v>
+        <v>111</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>103</v>
-      </c>
-      <c r="B96">
-        <v>4</v>
+        <v>111</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>103</v>
-      </c>
-      <c r="B97">
-        <v>3</v>
+        <v>111</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="B98">
-        <v>2</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>112</v>
+        <v>8</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="B99">
-        <v>1</v>
-      </c>
-      <c r="D99" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D99" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>112</v>
+      </c>
+      <c r="B100">
+        <v>6</v>
+      </c>
+      <c r="D100" t="s">
         <v>114</v>
-      </c>
-      <c r="B100">
-        <v>1</v>
-      </c>
-      <c r="C100" t="s">
-        <v>4</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B101">
-        <v>1</v>
-      </c>
-      <c r="C101" t="s">
-        <v>116</v>
-      </c>
-      <c r="D101" s="1">
-        <v>2018</v>
+        <v>5</v>
+      </c>
+      <c r="D101" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B102">
-        <v>5</v>
-      </c>
-      <c r="C102" t="s">
         <v>4</v>
       </c>
-      <c r="D102" s="1" t="s">
-        <v>119</v>
+      <c r="D102" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B103">
-        <v>5</v>
-      </c>
-      <c r="C103" t="s">
-        <v>116</v>
-      </c>
-      <c r="D103" s="1">
-        <v>2018</v>
+        <v>3</v>
+      </c>
+      <c r="D103" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B104">
-        <v>4</v>
-      </c>
-      <c r="C104" t="s">
-        <v>4</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>120</v>
+        <v>2</v>
+      </c>
+      <c r="D104" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B105">
-        <v>4</v>
-      </c>
-      <c r="C105" t="s">
-        <v>116</v>
-      </c>
-      <c r="D105" s="1">
-        <v>2017</v>
+        <v>1</v>
+      </c>
+      <c r="D105" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B106">
         <v>3</v>
       </c>
-      <c r="C106" t="s">
-        <v>4</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>121</v>
+      <c r="D106" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B107">
-        <v>3</v>
-      </c>
-      <c r="C107" t="s">
-        <v>116</v>
-      </c>
-      <c r="D107" s="1">
-        <v>2016</v>
+        <v>2</v>
+      </c>
+      <c r="D107" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B108">
-        <v>9</v>
-      </c>
-      <c r="C108" t="s">
-        <v>4</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>122</v>
+        <v>1</v>
+      </c>
+      <c r="D108" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>114</v>
-      </c>
-      <c r="B109">
-        <v>9</v>
-      </c>
-      <c r="C109" t="s">
-        <v>116</v>
-      </c>
-      <c r="D109" s="1">
-        <v>2014</v>
+        <v>126</v>
+      </c>
+      <c r="D109" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>114</v>
-      </c>
-      <c r="B110">
-        <v>10</v>
-      </c>
-      <c r="C110" t="s">
-        <v>4</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
+      </c>
+      <c r="D110" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>114</v>
-      </c>
-      <c r="B111">
-        <v>10</v>
-      </c>
-      <c r="C111" t="s">
-        <v>116</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>117</v>
+        <v>126</v>
+      </c>
+      <c r="D111" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>114</v>
-      </c>
-      <c r="B112">
-        <v>6</v>
-      </c>
-      <c r="C112" t="s">
-        <v>4</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
+      </c>
+      <c r="D112" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>114</v>
-      </c>
-      <c r="B113">
-        <v>6</v>
-      </c>
-      <c r="C113" t="s">
-        <v>116</v>
-      </c>
-      <c r="D113" s="1">
-        <v>2013</v>
+        <v>126</v>
+      </c>
+      <c r="D113" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>114</v>
-      </c>
-      <c r="B114">
-        <v>7</v>
-      </c>
-      <c r="C114" t="s">
-        <v>4</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>114</v>
-      </c>
-      <c r="B115">
-        <v>7</v>
-      </c>
-      <c r="C115" t="s">
-        <v>116</v>
-      </c>
-      <c r="D115">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>141</v>
-      </c>
-      <c r="D116" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>141</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>141</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>141</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>141</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>141</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>141</v>
-      </c>
-      <c r="D122" s="1" t="s">
+      <c r="D114" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>141</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>141</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>141</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>141</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>141</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>141</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>141</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>141</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>142</v>
-      </c>
-      <c r="B131">
-        <v>8</v>
-      </c>
-      <c r="D131" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>142</v>
-      </c>
-      <c r="B132">
-        <v>7</v>
-      </c>
-      <c r="D132" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>142</v>
-      </c>
-      <c r="B133">
-        <v>6</v>
-      </c>
-      <c r="D133" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>142</v>
-      </c>
-      <c r="B134">
-        <v>5</v>
-      </c>
-      <c r="D134" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>142</v>
-      </c>
-      <c r="B135">
-        <v>4</v>
-      </c>
-      <c r="D135" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>142</v>
-      </c>
-      <c r="B136">
-        <v>3</v>
-      </c>
-      <c r="D136" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>142</v>
-      </c>
-      <c r="B137">
-        <v>2</v>
-      </c>
-      <c r="D137" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>142</v>
-      </c>
-      <c r="B138">
-        <v>1</v>
-      </c>
-      <c r="D138" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>151</v>
-      </c>
-      <c r="B139">
-        <v>3</v>
-      </c>
-      <c r="D139" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>151</v>
-      </c>
-      <c r="B140">
-        <v>2</v>
-      </c>
-      <c r="D140" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>151</v>
-      </c>
-      <c r="B141">
-        <v>1</v>
-      </c>
-      <c r="D141" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>156</v>
-      </c>
-      <c r="D142" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>156</v>
-      </c>
-      <c r="D143" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>156</v>
-      </c>
-      <c r="D144" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>156</v>
-      </c>
-      <c r="D145" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>156</v>
-      </c>
-      <c r="D146" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>156</v>
-      </c>
-      <c r="D147" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>156</v>
-      </c>
-      <c r="D148" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>156</v>
-      </c>
-      <c r="D149" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>156</v>
-      </c>
-      <c r="D150" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>156</v>
-      </c>
-      <c r="D151" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>156</v>
-      </c>
-      <c r="D152" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>156</v>
-      </c>
-      <c r="D153" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>156</v>
-      </c>
-      <c r="D154" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>156</v>
-      </c>
-      <c r="D155" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>156</v>
-      </c>
-      <c r="D156" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>156</v>
-      </c>
-      <c r="D157" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>174</v>
-      </c>
-      <c r="D158" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>174</v>
-      </c>
-      <c r="D159" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>174</v>
-      </c>
-      <c r="D160" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>174</v>
-      </c>
-      <c r="D161" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>174</v>
-      </c>
-      <c r="D162" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>174</v>
-      </c>
-      <c r="D163" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CSS theming! Also bug fixes.
</commit_message>
<xml_diff>
--- a/example/cvdata.xlsx
+++ b/example/cvdata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="117">
   <si>
     <t>section</t>
   </si>
@@ -47,9 +47,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>nhuntington-klein@fullerton.edu</t>
-  </si>
-  <si>
     <t>phone</t>
   </si>
   <si>
@@ -65,15 +62,9 @@
     <t>twitter</t>
   </si>
   <si>
-    <t>nickchk</t>
-  </si>
-  <si>
     <t>github</t>
   </si>
   <si>
-    <t>NickCH-K</t>
-  </si>
-  <si>
     <t>employment</t>
   </si>
   <si>
@@ -357,6 +348,33 @@
   </si>
   <si>
     <t>"Human Capital vs. Signaling is Empirically Unresolvable." CSU Fullerton Department of Economics Working Paper 2018/010.</t>
+  </si>
+  <si>
+    <t>photo</t>
+  </si>
+  <si>
+    <t>![Profile](profile.jpg){width=130px}</t>
+  </si>
+  <si>
+    <t>[nickchk](https://twitter.com/nickchk)</t>
+  </si>
+  <si>
+    <t>[NickCH-K](https://github.com/NickCH-K)</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>Assistant Professor of Economics</t>
+  </si>
+  <si>
+    <t>institution</t>
+  </si>
+  <si>
+    <t>CSU Fullerton</t>
+  </si>
+  <si>
+    <t>[nhuntington-klein@fullerton.edu](mailto:nhuntington-klein@fullerton.edu)</t>
   </si>
 </sst>
 </file>
@@ -687,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -731,7 +749,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -739,10 +757,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>112</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -750,10 +768,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>114</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -761,10 +779,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -772,989 +790,1022 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8">
         <v>3</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>22</v>
+        <v>3</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" t="s">
-        <v>27</v>
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B14">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>8</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" t="s">
-        <v>37</v>
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B16">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>110</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B17">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B18">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B20">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" t="s">
         <v>26</v>
-      </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="C25" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D26" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B27">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B28">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B29">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D29" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>23</v>
+      </c>
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>102</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="B31">
-        <v>5</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>45</v>
+        <v>10</v>
+      </c>
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="B32">
-        <v>4</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>46</v>
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33">
-        <v>3</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
+      </c>
+      <c r="D33" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B36">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B37">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B38">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B39">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B40">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41">
+        <v>8</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B41">
-        <v>5</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B42">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B43">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>60</v>
+        <v>4</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47" t="s">
-        <v>63</v>
-      </c>
-      <c r="D47" s="1">
-        <v>2018</v>
+        <v>2</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B48">
-        <v>5</v>
-      </c>
-      <c r="C48" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>66</v>
+        <v>1</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B49">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>63</v>
-      </c>
-      <c r="D49" s="1">
-        <v>2018</v>
+        <v>4</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B50">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
+      </c>
+      <c r="D50" s="1">
+        <v>2018</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
         <v>4</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="D51" s="1">
-        <v>2017</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B52">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>4</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
+      </c>
+      <c r="D52" s="1">
+        <v>2018</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B53">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>63</v>
-      </c>
-      <c r="D53" s="1">
-        <v>2016</v>
+        <v>4</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B54">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>4</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
+      </c>
+      <c r="D54" s="1">
+        <v>2017</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B55">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>63</v>
-      </c>
-      <c r="D55" s="1">
-        <v>2014</v>
+        <v>4</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B56">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>4</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
+      </c>
+      <c r="D56" s="1">
+        <v>2016</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B57">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>63</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>64</v>
+        <v>4</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B58">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>4</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
+      </c>
+      <c r="D58" s="1">
+        <v>2014</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B59">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C59" t="s">
-        <v>63</v>
-      </c>
-      <c r="D59" s="1">
-        <v>2013</v>
+        <v>4</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>10</v>
+      </c>
+      <c r="C60" t="s">
+        <v>60</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B60">
-        <v>7</v>
-      </c>
-      <c r="C60" t="s">
-        <v>4</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B61">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>63</v>
-      </c>
-      <c r="D61">
-        <v>2011</v>
+        <v>4</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>88</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
+      </c>
+      <c r="B62">
+        <v>6</v>
+      </c>
+      <c r="C62" t="s">
+        <v>60</v>
+      </c>
+      <c r="D62" s="1">
+        <v>2013</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>88</v>
+        <v>58</v>
+      </c>
+      <c r="B63">
+        <v>7</v>
+      </c>
+      <c r="C63" t="s">
+        <v>4</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>88</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>75</v>
+        <v>58</v>
+      </c>
+      <c r="B64">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s">
+        <v>60</v>
+      </c>
+      <c r="D64">
+        <v>2011</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>89</v>
-      </c>
-      <c r="B77">
-        <v>8</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>97</v>
+        <v>85</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>89</v>
-      </c>
-      <c r="B78">
-        <v>7</v>
-      </c>
-      <c r="D78" t="s">
-        <v>90</v>
+        <v>85</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>89</v>
-      </c>
-      <c r="B79">
-        <v>6</v>
-      </c>
-      <c r="D79" t="s">
-        <v>91</v>
+        <v>85</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B80">
-        <v>5</v>
-      </c>
-      <c r="D80" t="s">
-        <v>92</v>
+        <v>8</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B81">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D81" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B82">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D82" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83">
+        <v>5</v>
+      </c>
+      <c r="D83" t="s">
         <v>89</v>
-      </c>
-      <c r="B83">
-        <v>2</v>
-      </c>
-      <c r="D83" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D84" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B85">
         <v>3</v>
       </c>
       <c r="D85" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B86">
         <v>2</v>
       </c>
       <c r="D86" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B87">
         <v>1</v>
       </c>
       <c r="D87" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>103</v>
+        <v>95</v>
+      </c>
+      <c r="B88">
+        <v>3</v>
       </c>
       <c r="D88" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>103</v>
+        <v>95</v>
+      </c>
+      <c r="B89">
+        <v>2</v>
       </c>
       <c r="D89" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>103</v>
+        <v>95</v>
+      </c>
+      <c r="B90">
+        <v>1</v>
       </c>
       <c r="D90" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D91" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D92" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>100</v>
+      </c>
+      <c r="D93" t="s">
         <v>103</v>
       </c>
-      <c r="D93" t="s">
-        <v>109</v>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>100</v>
+      </c>
+      <c r="D94" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>100</v>
+      </c>
+      <c r="D95" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>100</v>
+      </c>
+      <c r="D96" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Incorporated and tested CSS themes, and wrote instructions
</commit_message>
<xml_diff>
--- a/example/cvdata.xlsx
+++ b/example/cvdata.xlsx
@@ -332,9 +332,6 @@
     <t>The Potential Impact of Free Community College Programs with William Zumeta</t>
   </si>
   <si>
-    <t>Student Employment and Summer Bunching of Hours</t>
-  </si>
-  <si>
     <t>The Complexity of College Course Requirements with Rachel Baker</t>
   </si>
   <si>
@@ -375,6 +372,9 @@
   </si>
   <si>
     <t>[nhuntington-klein@fullerton.edu](mailto:nhuntington-klein@fullerton.edu)</t>
+  </si>
+  <si>
+    <t>Statistical Discrimination and Labor Market Competitiveness</t>
   </si>
 </sst>
 </file>
@@ -707,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,7 +749,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -757,10 +757,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" t="s">
         <v>112</v>
-      </c>
-      <c r="D4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -768,10 +768,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" t="s">
         <v>114</v>
-      </c>
-      <c r="D5" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -804,7 +804,7 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -815,7 +815,7 @@
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -823,10 +823,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" t="s">
         <v>108</v>
-      </c>
-      <c r="D10" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -937,7 +937,7 @@
         <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1773,7 +1773,7 @@
         <v>100</v>
       </c>
       <c r="D92" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -1781,7 +1781,7 @@
         <v>100</v>
       </c>
       <c r="D93" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -1789,7 +1789,7 @@
         <v>100</v>
       </c>
       <c r="D94" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -1797,7 +1797,7 @@
         <v>100</v>
       </c>
       <c r="D95" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -1805,7 +1805,7 @@
         <v>100</v>
       </c>
       <c r="D96" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>